<commit_message>
More work to Uranium ETF overview
</commit_message>
<xml_diff>
--- a/ETF Overview - Uranium.xlsx
+++ b/ETF Overview - Uranium.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4144A54D-AA62-4B3F-8E03-B59E85D47167}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B00AF42-59CB-4773-B302-394231F2AF2B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{23578CEB-2F1A-4001-95F2-BA0B39026A58}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Ticker</t>
   </si>
@@ -73,13 +73,94 @@
   </si>
   <si>
     <t>Sprott Uranium Physical Uranium Trust</t>
+  </si>
+  <si>
+    <t>£URNP</t>
+  </si>
+  <si>
+    <t>Sprott Uranium Miners UCITS ETF</t>
+  </si>
+  <si>
+    <t>LSE</t>
+  </si>
+  <si>
+    <t>$URNJ</t>
+  </si>
+  <si>
+    <t>Sprott Junior Uranium Miners ETF</t>
+  </si>
+  <si>
+    <t>NASDAQ</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Small Uranium miners, selected for potential for significant revenue &amp; asset growth</t>
+  </si>
+  <si>
+    <t>Holdings</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Inception</t>
+  </si>
+  <si>
+    <t>UCITS compliant version of $URNM</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Net Assets</t>
+  </si>
+  <si>
+    <t>Key Events</t>
+  </si>
+  <si>
+    <t>NUCL become third ETF offering exposure exposure to Uranium sector</t>
+  </si>
+  <si>
+    <t>$NLR</t>
+  </si>
+  <si>
+    <t>Uranium+Nuclear Energy ETF</t>
+  </si>
+  <si>
+    <t>SEMI-RELATED ETFS</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>CADUSD</t>
+  </si>
+  <si>
+    <t>TRUST-F</t>
+  </si>
+  <si>
+    <t>Sprott</t>
+  </si>
+  <si>
+    <t>Global X</t>
+  </si>
+  <si>
+    <t>Sector ETF Providers</t>
+  </si>
+  <si>
+    <t>2008(?)</t>
+  </si>
+  <si>
+    <t>VanEck</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,8 +187,29 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,6 +225,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -151,10 +271,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -171,9 +292,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -183,8 +301,43 @@
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -497,13 +650,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C917D1B-ACDD-498D-824B-3439F68C8C1A}">
-  <dimension ref="B2:M12"/>
+  <dimension ref="A2:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -513,10 +666,16 @@
     <col min="3" max="3" width="34.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" style="7"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="9.140625" style="4"/>
+    <col min="14" max="14" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="70.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -532,14 +691,26 @@
       <c r="F2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="H2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -549,21 +720,27 @@
       <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="10">
-        <v>22.1</v>
-      </c>
-      <c r="F3" s="11">
-        <f>E3*$F$12</f>
-        <v>18.343</v>
-      </c>
-      <c r="L3" s="5">
+      <c r="E3" s="9">
+        <v>21.49</v>
+      </c>
+      <c r="F3" s="10">
+        <f>E3*$I$28</f>
+        <v>17.836699999999997</v>
+      </c>
+      <c r="H3" s="11">
+        <v>1760</v>
+      </c>
+      <c r="J3" s="5">
         <v>4.3499999999999997E-2</v>
       </c>
-      <c r="M3" s="5">
+      <c r="K3" s="5">
         <v>0.30570000000000003</v>
       </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N3" s="14">
+        <v>40486</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -576,45 +753,265 @@
       <c r="E4" s="7">
         <v>35.130000000000003</v>
       </c>
-      <c r="F4" s="11">
-        <f>E4*$F$12</f>
+      <c r="F4" s="10">
+        <f>E4*$I$28</f>
         <v>29.157900000000001</v>
       </c>
-      <c r="L4" s="5">
+      <c r="H4" s="11">
+        <v>941.43</v>
+      </c>
+      <c r="J4" s="5">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="M4" s="5">
+      <c r="K4" s="5">
         <v>0.46279999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N4" s="14">
+        <v>43802</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="7">
+        <v>17.489999999999998</v>
+      </c>
+      <c r="F5" s="10">
+        <f>E5*$I$28</f>
+        <v>14.516699999999998</v>
+      </c>
+      <c r="H5" s="11">
+        <v>11.6</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" s="14">
+        <v>44958</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="10">
-        <v>13</v>
-      </c>
-      <c r="F5" s="11">
-        <f>E5*F12</f>
-        <v>10.79</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="E12" s="8" t="s">
+      <c r="E6" s="9">
+        <v>17.46</v>
+      </c>
+      <c r="F6" s="10">
+        <f>E6*I29*I28</f>
+        <v>10.723932</v>
+      </c>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="9">
+        <v>5.9279999999999999</v>
+      </c>
+      <c r="F8" s="10">
+        <f>E8</f>
+        <v>5.9279999999999999</v>
+      </c>
+      <c r="H8" s="12">
+        <f>51.7*(1+(1-I28))</f>
+        <v>60.488999999999997</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" s="14">
+        <v>44684</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="M10" s="21"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="9">
+        <v>56.24</v>
+      </c>
+      <c r="F11" s="10">
+        <f>E11*$I$28</f>
+        <v>46.679200000000002</v>
+      </c>
+      <c r="H11" s="11">
+        <v>57.63</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0.1007</v>
+      </c>
+      <c r="K11" s="5">
+        <v>5.96E-2</v>
+      </c>
+      <c r="N11" s="14">
+        <v>39307</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="M19" s="21"/>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N20" s="1">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N22" s="1">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="N27" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="O27" s="16"/>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="H28" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="9">
+      <c r="I28" s="8">
         <v>0.83</v>
       </c>
+      <c r="N28" s="17">
+        <v>44965</v>
+      </c>
+      <c r="O28" s="19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="H29" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="I29" s="8">
+        <v>0.74</v>
+      </c>
+      <c r="N29" s="18"/>
+      <c r="O29" s="19"/>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="N30" s="18"/>
+      <c r="O30" s="19"/>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="N31" s="18"/>
+      <c r="O31" s="19"/>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="N32" s="18"/>
+      <c r="O32" s="19"/>
+    </row>
+    <row r="33" spans="14:15" x14ac:dyDescent="0.2">
+      <c r="N33" s="18"/>
+      <c r="O33" s="19"/>
+    </row>
+    <row r="34" spans="14:15" x14ac:dyDescent="0.2">
+      <c r="N34" s="18"/>
+      <c r="O34" s="19"/>
+    </row>
+    <row r="35" spans="14:15" x14ac:dyDescent="0.2">
+      <c r="N35" s="18"/>
+      <c r="O35" s="19"/>
+    </row>
+    <row r="36" spans="14:15" x14ac:dyDescent="0.2">
+      <c r="N36" s="18"/>
+      <c r="O36" s="19"/>
+    </row>
+    <row r="37" spans="14:15" x14ac:dyDescent="0.2">
+      <c r="N37" s="18"/>
+      <c r="O37" s="19"/>
+    </row>
+    <row r="38" spans="14:15" x14ac:dyDescent="0.2">
+      <c r="N38" s="18"/>
+      <c r="O38" s="19"/>
+    </row>
+    <row r="39" spans="14:15" x14ac:dyDescent="0.2">
+      <c r="N39" s="18"/>
+      <c r="O39" s="19"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="N27:O27"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="M5" r:id="rId1" location=":~:text=United%20Kingdom-,Daily%20Holdings,-As%20of%202" xr:uid="{A02FF078-F82E-4D3E-9501-805C42D598FD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add some suppliers/producers to Uranium overview
</commit_message>
<xml_diff>
--- a/ETF Overview - Uranium.xlsx
+++ b/ETF Overview - Uranium.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F37B1B-CD87-459A-885F-9676BED7F9D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD4533F-CF94-4035-BA8B-F6FFD06EBEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{23578CEB-2F1A-4001-95F2-BA0B39026A58}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{23578CEB-2F1A-4001-95F2-BA0B39026A58}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
   <si>
     <t>Ticker</t>
   </si>
@@ -193,6 +202,30 @@
   </si>
   <si>
     <t>Extraction, Exploration etc. of Uranium &amp; other rare-earth metals</t>
+  </si>
+  <si>
+    <t>Uranium Producers/Suppliers</t>
+  </si>
+  <si>
+    <t>$CCJ</t>
+  </si>
+  <si>
+    <t>Cameco Corporation</t>
+  </si>
+  <si>
+    <t>£KAP</t>
+  </si>
+  <si>
+    <t>Kazatomprom</t>
+  </si>
+  <si>
+    <t>Worlds largest producer/supplier of natural uranium providing over 40% of global supply in 2019</t>
+  </si>
+  <si>
+    <t>Worlds second largest uranium producer, accounting for 18% of world production</t>
+  </si>
+  <si>
+    <t>NYSE</t>
   </si>
 </sst>
 </file>
@@ -371,15 +404,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -696,13 +729,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C917D1B-ACDD-498D-824B-3439F68C8C1A}">
-  <dimension ref="A2:O41"/>
+  <dimension ref="A2:O46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O19" sqref="O19"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -770,7 +803,7 @@
         <v>21.49</v>
       </c>
       <c r="F3" s="10">
-        <f>E3*$I$30</f>
+        <f>E3*$I$35</f>
         <v>17.836699999999997</v>
       </c>
       <c r="H3" s="11">
@@ -800,7 +833,7 @@
         <v>35.130000000000003</v>
       </c>
       <c r="F4" s="10">
-        <f>E4*$I$30</f>
+        <f>E4*$I$35</f>
         <v>29.157900000000001</v>
       </c>
       <c r="H4" s="11">
@@ -830,7 +863,7 @@
         <v>17.489999999999998</v>
       </c>
       <c r="F5" s="10">
-        <f>E5*$I$30</f>
+        <f>E5*$I$35</f>
         <v>14.516699999999998</v>
       </c>
       <c r="H5" s="11">
@@ -869,7 +902,7 @@
         <v>17.46</v>
       </c>
       <c r="F6" s="10">
-        <f>E6*I31*I30</f>
+        <f>E6*I36*I35</f>
         <v>10.723932</v>
       </c>
       <c r="H6" s="11"/>
@@ -892,7 +925,7 @@
         <v>5.9279999999999999</v>
       </c>
       <c r="H8" s="12">
-        <f>51.7*(1+(1-I30))</f>
+        <f>51.7*(1+(1-I35))</f>
         <v>60.488999999999997</v>
       </c>
       <c r="J8" s="15" t="s">
@@ -931,7 +964,7 @@
         <v>56.24</v>
       </c>
       <c r="F11" s="10">
-        <f>E11*$I$30</f>
+        <f>E11*$I$35</f>
         <v>46.679200000000002</v>
       </c>
       <c r="H11" s="11">
@@ -947,14 +980,14 @@
         <v>39307</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C14" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="M14" s="26"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="M14" s="25"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
@@ -997,118 +1030,175 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="2:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C21" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="25"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="M21" s="25"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="9">
+        <v>0.38950000000000001</v>
+      </c>
+      <c r="F22" s="10">
+        <f>E22</f>
+        <v>0.38950000000000001</v>
+      </c>
+      <c r="N22" s="4">
+        <v>1997</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="7">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="F23" s="10">
+        <f>E23*$I$35</f>
+        <v>33.366</v>
+      </c>
+      <c r="N23" s="4">
+        <v>1988</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="M21" s="20"/>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C22" s="1" t="s">
+      <c r="D26" s="20"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="M26" s="20"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C27" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="N22" s="1">
+      <c r="N27" s="1">
         <v>1981</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C23" s="1" t="s">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C28" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="N23" s="7" t="s">
+      <c r="N28" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C24" s="1" t="s">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C29" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="N24" s="1">
+      <c r="N29" s="1">
         <v>1955</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="G29" s="1" t="s">
+    <row r="34" spans="7:15" x14ac:dyDescent="0.2">
+      <c r="G34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H29" s="14">
+      <c r="H34" s="14">
         <v>44978</v>
       </c>
-      <c r="N29" s="24" t="s">
+      <c r="N34" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="O29" s="24"/>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="H30" s="23" t="s">
+      <c r="O34" s="27"/>
+    </row>
+    <row r="35" spans="7:15" x14ac:dyDescent="0.2">
+      <c r="H35" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="I30" s="8">
+      <c r="I35" s="8">
         <v>0.83</v>
       </c>
-      <c r="N30" s="17"/>
-      <c r="O30" s="18"/>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="H31" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="I31" s="8">
-        <v>0.74</v>
-      </c>
-      <c r="N31" s="17"/>
-      <c r="O31" s="18"/>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="N32" s="17"/>
-      <c r="O32" s="18"/>
-    </row>
-    <row r="33" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N33" s="17"/>
-      <c r="O33" s="18"/>
-    </row>
-    <row r="34" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N34" s="16">
-        <v>44965</v>
-      </c>
-      <c r="O34" s="18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="14:15" x14ac:dyDescent="0.2">
       <c r="N35" s="17"/>
       <c r="O35" s="18"/>
     </row>
-    <row r="36" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="7:15" x14ac:dyDescent="0.2">
+      <c r="H36" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I36" s="8">
+        <v>0.74</v>
+      </c>
       <c r="N36" s="17"/>
       <c r="O36" s="18"/>
     </row>
-    <row r="37" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="7:15" x14ac:dyDescent="0.2">
       <c r="N37" s="17"/>
       <c r="O37" s="18"/>
     </row>
-    <row r="38" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="7:15" x14ac:dyDescent="0.2">
       <c r="N38" s="17"/>
       <c r="O38" s="18"/>
     </row>
-    <row r="39" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N39" s="17"/>
-      <c r="O39" s="18"/>
-    </row>
-    <row r="40" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="7:15" x14ac:dyDescent="0.2">
+      <c r="N39" s="16">
+        <v>44965</v>
+      </c>
+      <c r="O39" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="7:15" x14ac:dyDescent="0.2">
       <c r="N40" s="17"/>
       <c r="O40" s="18"/>
     </row>
-    <row r="41" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="7:15" x14ac:dyDescent="0.2">
       <c r="N41" s="17"/>
       <c r="O41" s="18"/>
     </row>
+    <row r="42" spans="7:15" x14ac:dyDescent="0.2">
+      <c r="N42" s="17"/>
+      <c r="O42" s="18"/>
+    </row>
+    <row r="43" spans="7:15" x14ac:dyDescent="0.2">
+      <c r="N43" s="17"/>
+      <c r="O43" s="18"/>
+    </row>
+    <row r="44" spans="7:15" x14ac:dyDescent="0.2">
+      <c r="N44" s="17"/>
+      <c r="O44" s="18"/>
+    </row>
+    <row r="45" spans="7:15" x14ac:dyDescent="0.2">
+      <c r="N45" s="17"/>
+      <c r="O45" s="18"/>
+    </row>
+    <row r="46" spans="7:15" x14ac:dyDescent="0.2">
+      <c r="N46" s="17"/>
+      <c r="O46" s="18"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="N34:O34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M5" r:id="rId1" location=":~:text=United%20Kingdom-,Daily%20Holdings,-As%20of%202" xr:uid="{A02FF078-F82E-4D3E-9501-805C42D598FD}"/>

</xml_diff>